<commit_message>
Added flexibility for reading
</commit_message>
<xml_diff>
--- a/info/Proyecto.xlsx
+++ b/info/Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaqu\Documents\Codigo\Excel_to_prolog\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4857B9D7-B5F7-4A2D-871A-A8C7A56AF225}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072A9098-2963-4718-BF83-E305BE31AF70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-4332" windowWidth="30936" windowHeight="16896" xr2:uid="{EDDD431F-853B-824A-9AEB-247730D2FFD9}"/>
   </bookViews>
@@ -1306,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9791659-A9FA-8048-82D7-A664019D467A}">
   <dimension ref="A1:AL98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1445,7 +1445,7 @@
         <v>37</v>
       </c>
       <c r="F2" s="4">
-        <v>29390</v>
+        <v>29395</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>38</v>
@@ -1555,7 +1555,7 @@
         <v>37</v>
       </c>
       <c r="F3" s="4">
-        <v>16593</v>
+        <v>16598</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>40</v>
@@ -1657,7 +1657,7 @@
         <v>37</v>
       </c>
       <c r="F4" s="4">
-        <v>29392</v>
+        <v>29397</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>64</v>
@@ -1767,7 +1767,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="4">
-        <v>16628</v>
+        <v>16633</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>68</v>
@@ -1869,7 +1869,7 @@
         <v>37</v>
       </c>
       <c r="F6" s="4">
-        <v>16629</v>
+        <v>16634</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>68</v>
@@ -1971,7 +1971,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="4">
-        <v>16630</v>
+        <v>16635</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>68</v>
@@ -2073,7 +2073,7 @@
         <v>37</v>
       </c>
       <c r="F8" s="4">
-        <v>16600</v>
+        <v>16605</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>44</v>
@@ -2177,7 +2177,7 @@
         <v>37</v>
       </c>
       <c r="F9" s="4">
-        <v>16602</v>
+        <v>16607</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>44</v>
@@ -2281,7 +2281,7 @@
         <v>37</v>
       </c>
       <c r="F10" s="4">
-        <v>16603</v>
+        <v>16608</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>44</v>
@@ -2385,7 +2385,7 @@
         <v>37</v>
       </c>
       <c r="F11" s="4">
-        <v>16604</v>
+        <v>16609</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>44</v>
@@ -2489,7 +2489,7 @@
         <v>37</v>
       </c>
       <c r="F12" s="4">
-        <v>16597</v>
+        <v>16602</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>42</v>
@@ -2593,7 +2593,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="4">
-        <v>16598</v>
+        <v>16603</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>42</v>
@@ -2697,7 +2697,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="4">
-        <v>16599</v>
+        <v>16604</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>42</v>
@@ -2801,7 +2801,7 @@
         <v>37</v>
       </c>
       <c r="F15" s="4">
-        <v>29945</v>
+        <v>29950</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>50</v>
@@ -2905,7 +2905,7 @@
         <v>37</v>
       </c>
       <c r="F16" s="4">
-        <v>16633</v>
+        <v>16638</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>70</v>
@@ -3009,7 +3009,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="4">
-        <v>16606</v>
+        <v>16611</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>44</v>
@@ -3111,7 +3111,7 @@
         <v>37</v>
       </c>
       <c r="F18" s="4">
-        <v>20401</v>
+        <v>20406</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>96</v>
@@ -3213,7 +3213,7 @@
         <v>37</v>
       </c>
       <c r="F19" s="4">
-        <v>20404</v>
+        <v>20409</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>96</v>
@@ -3315,7 +3315,7 @@
         <v>37</v>
       </c>
       <c r="F20" s="4">
-        <v>20406</v>
+        <v>20411</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>96</v>
@@ -3417,7 +3417,7 @@
         <v>37</v>
       </c>
       <c r="F21" s="4">
-        <v>16608</v>
+        <v>16613</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>46</v>
@@ -3521,7 +3521,7 @@
         <v>37</v>
       </c>
       <c r="F22" s="4">
-        <v>16652</v>
+        <v>16657</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>78</v>
@@ -3625,7 +3625,7 @@
         <v>37</v>
       </c>
       <c r="F23" s="4">
-        <v>16653</v>
+        <v>16658</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>78</v>
@@ -3729,7 +3729,7 @@
         <v>37</v>
       </c>
       <c r="F24" s="4">
-        <v>16641</v>
+        <v>16646</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>78</v>
@@ -3833,7 +3833,7 @@
         <v>37</v>
       </c>
       <c r="F25" s="4">
-        <v>20399</v>
+        <v>20404</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>94</v>
@@ -3937,7 +3937,7 @@
         <v>37</v>
       </c>
       <c r="F26" s="4">
-        <v>29393</v>
+        <v>29398</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>82</v>
@@ -4049,7 +4049,7 @@
         <v>37</v>
       </c>
       <c r="F27" s="4">
-        <v>16665</v>
+        <v>16670</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>84</v>
@@ -4153,7 +4153,7 @@
         <v>37</v>
       </c>
       <c r="F28" s="4">
-        <v>16668</v>
+        <v>16673</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>84</v>
@@ -4257,7 +4257,7 @@
         <v>37</v>
       </c>
       <c r="F29" s="4">
-        <v>16658</v>
+        <v>16663</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>84</v>
@@ -4361,7 +4361,7 @@
         <v>37</v>
       </c>
       <c r="F30" s="4">
-        <v>16670</v>
+        <v>16675</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>86</v>
@@ -4465,7 +4465,7 @@
         <v>37</v>
       </c>
       <c r="F31" s="4">
-        <v>16644</v>
+        <v>16649</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>78</v>
@@ -4569,7 +4569,7 @@
         <v>37</v>
       </c>
       <c r="F32" s="4">
-        <v>16648</v>
+        <v>16653</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>78</v>
@@ -4673,7 +4673,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="4">
-        <v>16651</v>
+        <v>16656</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>78</v>
@@ -4777,7 +4777,7 @@
         <v>37</v>
       </c>
       <c r="F34" s="4">
-        <v>16622</v>
+        <v>16627</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>62</v>
@@ -4881,7 +4881,7 @@
         <v>37</v>
       </c>
       <c r="F35" s="4">
-        <v>16625</v>
+        <v>16630</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>66</v>
@@ -4985,7 +4985,7 @@
         <v>37</v>
       </c>
       <c r="F36" s="4">
-        <v>16626</v>
+        <v>16631</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>66</v>
@@ -5089,7 +5089,7 @@
         <v>37</v>
       </c>
       <c r="F37" s="4">
-        <v>16627</v>
+        <v>16632</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>66</v>
@@ -5193,7 +5193,7 @@
         <v>37</v>
       </c>
       <c r="F38" s="4">
-        <v>16639</v>
+        <v>16644</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>78</v>
@@ -5297,7 +5297,7 @@
         <v>37</v>
       </c>
       <c r="F39" s="4">
-        <v>16646</v>
+        <v>16651</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>78</v>
@@ -5401,7 +5401,7 @@
         <v>37</v>
       </c>
       <c r="F40" s="4">
-        <v>16654</v>
+        <v>16659</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>78</v>
@@ -5505,7 +5505,7 @@
         <v>37</v>
       </c>
       <c r="F41" s="4">
-        <v>16673</v>
+        <v>16678</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>90</v>
@@ -5609,7 +5609,7 @@
         <v>37</v>
       </c>
       <c r="F42" s="4">
-        <v>16636</v>
+        <v>16641</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>74</v>
@@ -5713,7 +5713,7 @@
         <v>37</v>
       </c>
       <c r="F43" s="4">
-        <v>16637</v>
+        <v>16642</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>74</v>
@@ -5817,7 +5817,7 @@
         <v>37</v>
       </c>
       <c r="F44" s="4">
-        <v>20400</v>
+        <v>20405</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>96</v>
@@ -5921,7 +5921,7 @@
         <v>37</v>
       </c>
       <c r="F45" s="4">
-        <v>20402</v>
+        <v>20407</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>96</v>
@@ -6025,7 +6025,7 @@
         <v>37</v>
       </c>
       <c r="F46" s="4">
-        <v>20403</v>
+        <v>20408</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>96</v>
@@ -6129,7 +6129,7 @@
         <v>37</v>
       </c>
       <c r="F47" s="4">
-        <v>16618</v>
+        <v>16623</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>60</v>
@@ -6233,7 +6233,7 @@
         <v>37</v>
       </c>
       <c r="F48" s="4">
-        <v>16619</v>
+        <v>16624</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>60</v>
@@ -6337,7 +6337,7 @@
         <v>37</v>
       </c>
       <c r="F49" s="4">
-        <v>16620</v>
+        <v>16625</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>60</v>
@@ -6441,7 +6441,7 @@
         <v>37</v>
       </c>
       <c r="F50" s="4">
-        <v>16621</v>
+        <v>16626</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>60</v>
@@ -6545,7 +6545,7 @@
         <v>37</v>
       </c>
       <c r="F51" s="4">
-        <v>16601</v>
+        <v>16606</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>44</v>
@@ -6645,7 +6645,7 @@
         <v>37</v>
       </c>
       <c r="F52" s="4">
-        <v>16605</v>
+        <v>16610</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>44</v>
@@ -6745,7 +6745,7 @@
         <v>37</v>
       </c>
       <c r="F53" s="4">
-        <v>16624</v>
+        <v>16629</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>62</v>
@@ -6845,7 +6845,7 @@
         <v>37</v>
       </c>
       <c r="F54" s="4">
-        <v>20407</v>
+        <v>20412</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>96</v>
@@ -6945,7 +6945,7 @@
         <v>37</v>
       </c>
       <c r="F55" s="4">
-        <v>16663</v>
+        <v>16668</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>84</v>
@@ -7049,7 +7049,7 @@
         <v>37</v>
       </c>
       <c r="F56" s="4">
-        <v>16660</v>
+        <v>16665</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>84</v>
@@ -7153,7 +7153,7 @@
         <v>37</v>
       </c>
       <c r="F57" s="4">
-        <v>16661</v>
+        <v>16666</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>84</v>
@@ -7257,7 +7257,7 @@
         <v>37</v>
       </c>
       <c r="F58" s="4">
-        <v>16638</v>
+        <v>16643</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>76</v>
@@ -7361,7 +7361,7 @@
         <v>37</v>
       </c>
       <c r="F59" s="4">
-        <v>16655</v>
+        <v>16660</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>80</v>
@@ -7473,7 +7473,7 @@
         <v>37</v>
       </c>
       <c r="F60" s="4">
-        <v>16662</v>
+        <v>16667</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>84</v>
@@ -7577,7 +7577,7 @@
         <v>37</v>
       </c>
       <c r="F61" s="4">
-        <v>16677</v>
+        <v>16682</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>92</v>
@@ -7681,7 +7681,7 @@
         <v>37</v>
       </c>
       <c r="F62" s="4">
-        <v>16678</v>
+        <v>16683</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>92</v>
@@ -7785,7 +7785,7 @@
         <v>37</v>
       </c>
       <c r="F63" s="4">
-        <v>16613</v>
+        <v>16618</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>56</v>
@@ -7887,7 +7887,7 @@
         <v>37</v>
       </c>
       <c r="F64" s="4">
-        <v>16614</v>
+        <v>16619</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>56</v>
@@ -7989,7 +7989,7 @@
         <v>37</v>
       </c>
       <c r="F65" s="4">
-        <v>16615</v>
+        <v>16620</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>56</v>
@@ -8091,7 +8091,7 @@
         <v>37</v>
       </c>
       <c r="F66" s="4">
-        <v>16650</v>
+        <v>16655</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>78</v>
@@ -8195,7 +8195,7 @@
         <v>37</v>
       </c>
       <c r="F67" s="4">
-        <v>16666</v>
+        <v>16671</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>84</v>
@@ -8299,7 +8299,7 @@
         <v>37</v>
       </c>
       <c r="F68" s="4">
-        <v>16667</v>
+        <v>16672</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>84</v>
@@ -8403,7 +8403,7 @@
         <v>37</v>
       </c>
       <c r="F69" s="4">
-        <v>16664</v>
+        <v>16669</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>84</v>
@@ -8507,7 +8507,7 @@
         <v>37</v>
       </c>
       <c r="F70" s="4">
-        <v>16659</v>
+        <v>16664</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>84</v>
@@ -8611,7 +8611,7 @@
         <v>37</v>
       </c>
       <c r="F71" s="4">
-        <v>16669</v>
+        <v>16674</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>86</v>
@@ -8715,7 +8715,7 @@
         <v>37</v>
       </c>
       <c r="F72" s="4">
-        <v>16674</v>
+        <v>16679</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>92</v>
@@ -8819,7 +8819,7 @@
         <v>37</v>
       </c>
       <c r="F73" s="4">
-        <v>16675</v>
+        <v>16680</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>92</v>
@@ -8923,7 +8923,7 @@
         <v>37</v>
       </c>
       <c r="F74" s="4">
-        <v>16607</v>
+        <v>16612</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>46</v>
@@ -9027,7 +9027,7 @@
         <v>37</v>
       </c>
       <c r="F75" s="4">
-        <v>16609</v>
+        <v>16614</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>52</v>
@@ -9131,7 +9131,7 @@
         <v>37</v>
       </c>
       <c r="F76" s="4">
-        <v>16623</v>
+        <v>16628</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>62</v>
@@ -9235,7 +9235,7 @@
         <v>37</v>
       </c>
       <c r="F77" s="4">
-        <v>20405</v>
+        <v>20410</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>96</v>
@@ -9339,7 +9339,7 @@
         <v>37</v>
       </c>
       <c r="F78" s="4">
-        <v>16595</v>
+        <v>16600</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>40</v>
@@ -9441,7 +9441,7 @@
         <v>37</v>
       </c>
       <c r="F79" s="4">
-        <v>16596</v>
+        <v>16601</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>40</v>
@@ -9543,7 +9543,7 @@
         <v>37</v>
       </c>
       <c r="F80" s="4">
-        <v>16634</v>
+        <v>16639</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>72</v>
@@ -9645,7 +9645,7 @@
         <v>37</v>
       </c>
       <c r="F81" s="4">
-        <v>16635</v>
+        <v>16640</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>72</v>
@@ -9747,7 +9747,7 @@
         <v>37</v>
       </c>
       <c r="F82" s="4">
-        <v>16642</v>
+        <v>16647</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>78</v>
@@ -9851,7 +9851,7 @@
         <v>37</v>
       </c>
       <c r="F83" s="4">
-        <v>16645</v>
+        <v>16650</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>78</v>
@@ -9955,7 +9955,7 @@
         <v>37</v>
       </c>
       <c r="F84" s="4">
-        <v>16649</v>
+        <v>16654</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>78</v>
@@ -10059,7 +10059,7 @@
         <v>37</v>
       </c>
       <c r="F85" s="4">
-        <v>16656</v>
+        <v>16661</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>84</v>
@@ -10163,7 +10163,7 @@
         <v>37</v>
       </c>
       <c r="F86" s="4">
-        <v>16616</v>
+        <v>16621</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>58</v>
@@ -10265,7 +10265,7 @@
         <v>37</v>
       </c>
       <c r="F87" s="4">
-        <v>16617</v>
+        <v>16622</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>58</v>
@@ -10367,7 +10367,7 @@
         <v>37</v>
       </c>
       <c r="F88" s="4">
-        <v>16631</v>
+        <v>16636</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>70</v>
@@ -10469,7 +10469,7 @@
         <v>37</v>
       </c>
       <c r="F89" s="4">
-        <v>16632</v>
+        <v>16637</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>70</v>
@@ -10571,7 +10571,7 @@
         <v>37</v>
       </c>
       <c r="F90" s="4">
-        <v>16594</v>
+        <v>16599</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>40</v>
@@ -10673,7 +10673,7 @@
         <v>37</v>
       </c>
       <c r="F91" s="4">
-        <v>29391</v>
+        <v>29396</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>48</v>
@@ -10783,7 +10783,7 @@
         <v>37</v>
       </c>
       <c r="F92" s="4">
-        <v>16611</v>
+        <v>16616</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>54</v>
@@ -10885,7 +10885,7 @@
         <v>37</v>
       </c>
       <c r="F93" s="4">
-        <v>16610</v>
+        <v>16615</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>54</v>
@@ -10987,7 +10987,7 @@
         <v>37</v>
       </c>
       <c r="F94" s="4">
-        <v>16612</v>
+        <v>16617</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>54</v>
@@ -11089,7 +11089,7 @@
         <v>37</v>
       </c>
       <c r="F95" s="4">
-        <v>16643</v>
+        <v>16648</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>78</v>
@@ -11193,7 +11193,7 @@
         <v>37</v>
       </c>
       <c r="F96" s="4">
-        <v>16647</v>
+        <v>16652</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>78</v>
@@ -11297,7 +11297,7 @@
         <v>37</v>
       </c>
       <c r="F97" s="4">
-        <v>16671</v>
+        <v>16676</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>88</v>
@@ -11401,7 +11401,7 @@
         <v>37</v>
       </c>
       <c r="F98" s="4">
-        <v>16672</v>
+        <v>16677</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>90</v>

</xml_diff>